<commit_message>
added get_result and test for get_result
</commit_message>
<xml_diff>
--- a/example_excel.xlsx
+++ b/example_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikm\Desktop\automatic_wisc_repport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikm\Desktop\automatic_wisc_rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E08DB35-5A5C-4374-A91A-DA1D6FDD097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF51F82-79E3-40E3-A6E2-32C7EF03605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F38C289D-5300-4E84-914E-C5B6863138AF}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -490,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added general description of scores + test
</commit_message>
<xml_diff>
--- a/example_excel.xlsx
+++ b/example_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikm\Desktop\automatic_wisc_rapport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikm\Ecco\automatic_wisc_rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF51F82-79E3-40E3-A6E2-32C7EF03605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E2962B-FFA9-4B5F-8EFC-89D4BEB4F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F38C289D-5300-4E84-914E-C5B6863138AF}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="21840" xr2:uid="{F38C289D-5300-4E84-914E-C5B6863138AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,12 +438,12 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,88 +457,88 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
       </c>
       <c r="B4">
         <v>86</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>116</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>130</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>